<commit_message>
updated results upper segria sud
</commit_message>
<xml_diff>
--- a/main/results/SegriaSud/Upper/gridTurb.xlsx
+++ b/main/results/SegriaSud/Upper/gridTurb.xlsx
@@ -115,7 +115,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -125,6 +125,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -200,7 +204,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart59.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -321,25 +325,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>64.3976712328767</c:v>
+                  <c:v>-54.7804109589041</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.0617808219178</c:v>
+                  <c:v>-55.3902739726027</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-16.5341095890411</c:v>
+                  <c:v>-56.2601369863014</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-48.6008219178082</c:v>
+                  <c:v>-56.5460273972603</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-52.5704109589041</c:v>
+                  <c:v>-56.5430136986301</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-54.8361643835616</c:v>
+                  <c:v>-56.4252054794521</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-56.0178082191781</c:v>
+                  <c:v>-56.0972602739726</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>-56.1</c:v>
@@ -349,11 +353,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="56976877"/>
-        <c:axId val="6707904"/>
+        <c:axId val="54991119"/>
+        <c:axId val="37878823"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56976877"/>
+        <c:axId val="54991119"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -381,12 +385,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6707904"/>
+        <c:crossAx val="37878823"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="6707904"/>
+        <c:axId val="37878823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -423,7 +427,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56976877"/>
+        <c:crossAx val="54991119"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -471,7 +475,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart60.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -621,11 +625,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="18797388"/>
-        <c:axId val="62352980"/>
+        <c:axId val="82490165"/>
+        <c:axId val="44830681"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="18797388"/>
+        <c:axId val="82490165"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,12 +657,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62352980"/>
+        <c:crossAx val="44830681"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62352980"/>
+        <c:axId val="44830681"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -695,7 +699,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18797388"/>
+        <c:crossAx val="82490165"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -747,16 +751,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>49680</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>585000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>684000</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>405360</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>123840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -764,8 +768,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4113720" y="210600"/>
-        <a:ext cx="6323760" cy="2907000"/>
+        <a:off x="10338480" y="143640"/>
+        <a:ext cx="6323040" cy="2906280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -777,16 +781,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>78840</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>624240</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>144360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>713160</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>444600</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -794,8 +798,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4142880" y="3251880"/>
-        <a:ext cx="6323760" cy="2907000"/>
+        <a:off x="10377720" y="3070440"/>
+        <a:ext cx="6323040" cy="2906280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -816,7 +820,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -826,11 +830,11 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="n">
-        <v>6000</v>
+        <v>200</v>
       </c>
       <c r="C1" s="1" t="n">
         <f aca="false">B1/20/365</f>
-        <v>0.821917808219178</v>
+        <v>0.0273972602739726</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -856,11 +860,11 @@
       </c>
       <c r="C4" s="2" t="n">
         <f aca="false">A4*$C$1</f>
-        <v>123.287671232877</v>
+        <v>4.10958904109589</v>
       </c>
       <c r="D4" s="2" t="n">
         <f aca="false">B4+C4</f>
-        <v>64.3976712328767</v>
+        <v>-54.7804109589041</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -872,11 +876,11 @@
       </c>
       <c r="C5" s="2" t="n">
         <f aca="false">A5*$C$1</f>
-        <v>82.1917808219178</v>
+        <v>2.73972602739726</v>
       </c>
       <c r="D5" s="2" t="n">
         <f aca="false">B5+C5</f>
-        <v>24.0617808219178</v>
+        <v>-55.3902739726027</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -888,11 +892,11 @@
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">A6*$C$1</f>
-        <v>41.0958904109589</v>
+        <v>1.36986301369863</v>
       </c>
       <c r="D6" s="2" t="n">
         <f aca="false">B6+C6</f>
-        <v>-16.5341095890411</v>
+        <v>-56.2601369863014</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -904,66 +908,66 @@
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">A7*$C$1</f>
-        <v>8.21917808219178</v>
+        <v>0.273972602739726</v>
       </c>
       <c r="D7" s="2" t="n">
         <f aca="false">B7+C7</f>
-        <v>-48.6008219178082</v>
+        <v>-56.5460273972603</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="3" t="n">
         <v>-56.68</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">A8*$C$1</f>
-        <v>4.10958904109589</v>
+        <v>0.136986301369863</v>
       </c>
       <c r="D8" s="2" t="n">
         <f aca="false">B8+C8</f>
-        <v>-52.5704109589041</v>
+        <v>-56.5430136986301</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="3" t="n">
         <v>-56.48</v>
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">A9*$C$1</f>
-        <v>1.64383561643836</v>
+        <v>0.0547945205479452</v>
       </c>
       <c r="D9" s="2" t="n">
         <f aca="false">B9+C9</f>
-        <v>-54.8361643835616</v>
+        <v>-56.4252054794521</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="3" t="n">
         <v>0.1</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="3" t="n">
         <v>-56.1</v>
       </c>
       <c r="C10" s="2" t="n">
         <f aca="false">A10*$C$1</f>
-        <v>0.0821917808219178</v>
+        <v>0.00273972602739726</v>
       </c>
       <c r="D10" s="2" t="n">
         <f aca="false">B10+C10</f>
-        <v>-56.0178082191781</v>
+        <v>-56.0972602739726</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="3" t="n">
         <v>-56.1</v>
       </c>
       <c r="C11" s="2" t="n">

</xml_diff>